<commit_message>
Second commit Login Test added
</commit_message>
<xml_diff>
--- a/src/test/java/com/mystore/testcases/Sachin.xlsx
+++ b/src/test/java/com/mystore/testcases/Sachin.xlsx
@@ -16,35 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>lname</t>
-  </si>
-  <si>
     <t>passward</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>sachin125@gmail.com</t>
   </si>
   <si>
-    <t>sachin1225@gmail.com</t>
-  </si>
-  <si>
     <t>sachin1452@gmail.com</t>
   </si>
   <si>
@@ -63,54 +45,6 @@
     <t>sachin112545@gmail.com</t>
   </si>
   <si>
-    <t>Sachin</t>
-  </si>
-  <si>
-    <t>ajay</t>
-  </si>
-  <si>
-    <t>dinl</t>
-  </si>
-  <si>
-    <t>mjlkdi</t>
-  </si>
-  <si>
-    <t>ghsdgag</t>
-  </si>
-  <si>
-    <t>bhvjfjusd</t>
-  </si>
-  <si>
-    <t>gfyj</t>
-  </si>
-  <si>
-    <t>gffuy</t>
-  </si>
-  <si>
-    <t>fyagfka</t>
-  </si>
-  <si>
-    <t>asa</t>
-  </si>
-  <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>ascascfew</t>
-  </si>
-  <si>
-    <t>xce</t>
-  </si>
-  <si>
-    <t>csd</t>
-  </si>
-  <si>
-    <t>sadqw</t>
-  </si>
-  <si>
-    <t>sda</t>
-  </si>
-  <si>
     <t>dfsa455</t>
   </si>
   <si>
@@ -133,6 +67,9 @@
   </si>
   <si>
     <t>dhsgfb25488</t>
+  </si>
+  <si>
+    <t>sachin12257@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -477,224 +414,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5">
-        <v>25</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7">
-        <v>25</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8">
-        <v>25</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9">
-        <v>25</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <v>2011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>